<commit_message>
Added 2 more example test cases
</commit_message>
<xml_diff>
--- a/Test_cases.xlsx
+++ b/Test_cases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patry\OneDrive\Pulpit\Programowanie\Testowanie_oprogramowania\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patry\OneDrive\Pulpit\Programowanie\manual_testing_my_proj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410DA5BE-1DB1-46C6-88D2-D5356399D291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4489CDA9-E601-4093-9C28-517F3AD86729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{24E67711-1C86-4EBF-B128-13D4585E305B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -122,6 +122,39 @@
   </si>
   <si>
     <t>Displayed message: "Usunięto: „Postcard V1”. Cofnij?"</t>
+  </si>
+  <si>
+    <t>Correct product search</t>
+  </si>
+  <si>
+    <t>Poster V1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open the website https://test.testowanie-oprogramowania.pl
+2. Press the Shop tab
+3. Insert into "Search products…" field the input value
+4.Press the search button to the left of the field
+</t>
+  </si>
+  <si>
+    <t>Redirection to the product page</t>
+  </si>
+  <si>
+    <t>Invalid coupon code</t>
+  </si>
+  <si>
+    <t>xyz321u5s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open the website https://test.testowanie-oprogramowania.pl
+2. Press the Shopping cart tab
+3. Press the "Zobacz koszyk" button
+4.Insert into "Kod kuponu" field input value
+5. Press the "Wykorzystaj kupon" button
+</t>
+  </si>
+  <si>
+    <t>Displayed message: "Kupon "xyz321u5s" nie istnieje!"</t>
   </si>
 </sst>
 </file>
@@ -199,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -215,6 +248,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -552,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22D80943-52C7-40E7-9F31-36A5AADFB35B}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -561,8 +597,8 @@
     <col min="1" max="1" width="36.6640625" customWidth="1"/>
     <col min="2" max="2" width="32.109375" customWidth="1"/>
     <col min="3" max="3" width="28.44140625" customWidth="1"/>
-    <col min="4" max="4" width="32.5546875" customWidth="1"/>
-    <col min="5" max="5" width="44.6640625" customWidth="1"/>
+    <col min="4" max="4" width="34.6640625" customWidth="1"/>
+    <col min="5" max="5" width="49.21875" customWidth="1"/>
     <col min="6" max="6" width="19.21875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -596,7 +632,7 @@
       <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="4" t="s">
@@ -606,7 +642,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="108.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="122.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -616,7 +652,7 @@
       <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="8" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="7" t="s">
@@ -626,7 +662,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="93.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="114" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
@@ -636,7 +672,7 @@
       <c r="C4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="8" t="s">
         <v>19</v>
       </c>
       <c r="E4" t="s">
@@ -646,7 +682,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="82.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="113.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
@@ -656,7 +692,7 @@
       <c r="C5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="8" t="s">
         <v>20</v>
       </c>
       <c r="E5" t="s">
@@ -666,17 +702,45 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+    <row r="6" spans="1:6" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="153.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>

</xml_diff>